<commit_message>
Updated data with corrected encoding
</commit_message>
<xml_diff>
--- a/data/Liga.xlsx
+++ b/data/Liga.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L-Blu\Levi\Programmieren\Python\DBB-Widgets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L-Blu\Levi\Programmieren\Python\DBB_Widgets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3881F154-4EDD-49EF-8A3E-7A9C01731FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B610D0B-460E-43A9-ACF3-01123F6919A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Liga" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
-  <si>
-    <t>Index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -58,7 +55,7 @@
     <t xml:space="preserve"> Senioren</t>
   </si>
   <si>
-    <t xml:space="preserve"> Vorbereitungsspiele (ByLH-PRE)</t>
+    <t xml:space="preserve">  (U) Vorbereitungsspiele (ByLH-PRE)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;div id="widget_1728459670409"&gt;&lt;/div&gt;         &lt;script&gt;                 widget.ligawidget('widget_1728459670409',                         {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":true,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"ligaNr":"20098","vereinsId":"977","rangeDays":8,"activeTap":"tabelle","tapColorActive":"FFFFFF","tapBgColorActive":"000000","tapBorderColorActive":"00CC00","colorTableHeader":"666666","bgColorTableHeader":"F0F0F0","colorTableListItem":"000000","bgColorTableListItem":"FFFFFF","colorTableListItem2":"000000","bgColorTableListItem2":"FFFFFF","showKuerzelInTabelle":false});         &lt;/script&gt;     </t>
@@ -286,7 +283,7 @@
     <t xml:space="preserve">    &lt;div id="widget_1728459673787"&gt;&lt;/div&gt;         &lt;script&gt;                 widget.ligawidget('widget_1728459673787',                         {"iframeWidth":600,"iframeHeight":600,"showRefreshButton":true,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"ligaNr":"210054","vereinsId":"977","rangeDays":8,"activeTap":"tabelle","tapColorActive":"FFFFFF","tapBgColorActive":"000000","tapBorderColorActive":"00CC00","colorTableHeader":"666666","bgColorTableHeader":"F0F0F0","colorTableListItem":"000000","bgColorTableListItem":"FFFFFF","colorTableListItem2":"000000","bgColorTableListItem2":"FFFFFF","showKuerzelInTabelle":false});         &lt;/script&gt;     </t>
   </si>
   <si>
-    <t xml:space="preserve"> Bezirksoberliga u10 (u10bol) 2024/25</t>
+    <t xml:space="preserve"> Bezirksoberliga u10 wbl (bolu10w) 2024/25</t>
   </si>
   <si>
     <t xml:space="preserve">    &lt;div id="widget_1728459673970"&gt;&lt;/div&gt;         &lt;script&gt;                 widget.ligawidget('widget_1728459673970',                         {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":true,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"ligaNr":"210055","vereinsId":"977","rangeDays":8,"activeTap":"tabelle","tapColorActive":"FFFFFF","tapBgColorActive":"000000","tapBorderColorActive":"00CC00","colorTableHeader":"666666","bgColorTableHeader":"F0F0F0","colorTableListItem":"000000","bgColorTableListItem":"FFFFFF","colorTableListItem2":"000000","bgColorTableListItem2":"FFFFFF","showKuerzelInTabelle":false});         &lt;/script&gt;     </t>
@@ -304,52 +301,73 @@
     <t xml:space="preserve">    &lt;div id="widget_1728459674122"&gt;&lt;/div&gt;         &lt;script&gt;                 widget.ligawidget('widget_1728459674122',                         {"iframeWidth":600,"iframeHeight":600,"showRefreshButton":true,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"ligaNr":"21122","vereinsId":"977","rangeDays":8,"activeTap":"tabelle","tapColorActive":"FFFFFF","tapBgColorActive":"000000","tapBorderColorActive":"00CC00","colorTableHeader":"666666","bgColorTableHeader":"F0F0F0","colorTableListItem":"000000","bgColorTableListItem":"FFFFFF","colorTableListItem2":"000000","bgColorTableListItem2":"FFFFFF","showKuerzelInTabelle":false});         &lt;/script&gt;</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> männlich</t>
+  </si>
+  <si>
+    <t>ä</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK SB München</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK SB München 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bayernliga Herren Süd (ByLHS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK SB München (2RL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK SB München 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK SB München 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Regionalliga Süd (2RLS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJK Sportbund München</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bayernliga U16 männlich Süd</t>
+  </si>
+  <si>
+    <t>(zurückgezogen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Landesliga U14 männlich Süd</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>Ü</t>
+  </si>
+  <si>
     <t>Code groß</t>
   </si>
   <si>
-    <t xml:space="preserve"> männlich</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK SB München</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK SB München 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bayernliga Herren Süd (ByLHS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK SB München (2RL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK SB München 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK SB München 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2. Regionalliga Süd (2RLS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DJK Sportbund München</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bayernliga U16 männlich Süd</t>
-  </si>
-  <si>
-    <t>(zurückgezogen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Landesliga U14 männlich Süd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>ß</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -827,9 +845,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1184,29 +1201,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E29" sqref="C27:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1231,929 +1235,807 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>20098</v>
+      </c>
+      <c r="H2">
+        <v>1728459670409</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
-      </c>
-      <c r="H2">
-        <v>20098</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1728459670409</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3">
         <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="G3">
+        <v>20006</v>
       </c>
       <c r="H3">
-        <v>20006</v>
-      </c>
-      <c r="I3" s="1">
         <v>1728459670646</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="L3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>20100</v>
+      </c>
+      <c r="H4">
+        <v>1728459670841</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
-      </c>
-      <c r="H4">
-        <v>20100</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1728459670841</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>21102</v>
+      </c>
+      <c r="H5">
+        <v>1728459671002</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
-      </c>
-      <c r="H5">
-        <v>21102</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1728459671002</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="K5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="L5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>21103</v>
+      </c>
+      <c r="H6">
+        <v>1728459671162</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
-      </c>
-      <c r="H6">
-        <v>21103</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1728459671162</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>299</v>
+      </c>
+      <c r="H7">
+        <v>1728459671332</v>
+      </c>
+      <c r="I7" t="s">
         <v>30</v>
-      </c>
-      <c r="H7">
-        <v>299</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1728459671332</v>
       </c>
       <c r="J7" t="s">
         <v>31</v>
       </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8">
+        <v>202</v>
+      </c>
+      <c r="H8">
+        <v>1728459671487</v>
+      </c>
+      <c r="I8" t="s">
         <v>32</v>
-      </c>
-      <c r="L7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H8">
-        <v>202</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1728459671487</v>
       </c>
       <c r="J8" t="s">
         <v>33</v>
       </c>
-      <c r="K8" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
-      </c>
-      <c r="L8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
       </c>
       <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>210056</v>
+      </c>
+      <c r="H9">
+        <v>1728459671665</v>
+      </c>
+      <c r="I9" t="s">
         <v>37</v>
-      </c>
-      <c r="H9">
-        <v>210056</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1728459671665</v>
       </c>
       <c r="J9" t="s">
         <v>38</v>
       </c>
-      <c r="K9" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="L9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>210046</v>
+      </c>
+      <c r="H10">
+        <v>1728459671821</v>
+      </c>
+      <c r="I10" t="s">
         <v>41</v>
-      </c>
-      <c r="H10">
-        <v>210046</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1728459671821</v>
       </c>
       <c r="J10" t="s">
         <v>42</v>
       </c>
-      <c r="K10" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="L10" t="s">
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G11">
+        <v>20168</v>
+      </c>
+      <c r="H11">
+        <v>1728459671967</v>
+      </c>
+      <c r="I11" t="s">
         <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11">
-        <v>20168</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1728459671967</v>
       </c>
       <c r="J11" t="s">
         <v>45</v>
       </c>
-      <c r="K11" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" t="s">
         <v>46</v>
       </c>
-      <c r="L11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>210048</v>
+      </c>
+      <c r="H12">
+        <v>1728459672117</v>
+      </c>
+      <c r="I12" t="s">
         <v>47</v>
-      </c>
-      <c r="H12">
-        <v>210048</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1728459672117</v>
       </c>
       <c r="J12" t="s">
         <v>48</v>
       </c>
-      <c r="K12" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="L12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>21109</v>
+      </c>
+      <c r="H13">
+        <v>1728459672266</v>
+      </c>
+      <c r="I13" t="s">
         <v>50</v>
-      </c>
-      <c r="H13">
-        <v>21109</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1728459672266</v>
       </c>
       <c r="J13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
         <v>52</v>
-      </c>
-      <c r="L13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>53</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14">
+        <v>21126</v>
+      </c>
+      <c r="H14">
+        <v>1728459672414</v>
+      </c>
+      <c r="I14" t="s">
         <v>54</v>
-      </c>
-      <c r="H14">
-        <v>21126</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1728459672414</v>
       </c>
       <c r="J14" t="s">
         <v>55</v>
       </c>
-      <c r="K14" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="L14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>40</v>
-      </c>
       <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>210051</v>
+      </c>
+      <c r="H15">
+        <v>1728459672564</v>
+      </c>
+      <c r="I15" t="s">
         <v>58</v>
-      </c>
-      <c r="H15">
-        <v>210051</v>
-      </c>
-      <c r="I15" s="1">
-        <v>1728459672564</v>
       </c>
       <c r="J15" t="s">
         <v>59</v>
       </c>
-      <c r="K15" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="L15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
       <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>21119</v>
+      </c>
+      <c r="H16">
+        <v>1728459672714</v>
+      </c>
+      <c r="I16" t="s">
         <v>62</v>
-      </c>
-      <c r="H16">
-        <v>21119</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1728459672714</v>
       </c>
       <c r="J16" t="s">
         <v>63</v>
       </c>
-      <c r="K16" t="s">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
         <v>64</v>
       </c>
-      <c r="L16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>21112</v>
+      </c>
+      <c r="H17">
+        <v>1728459672865</v>
+      </c>
+      <c r="I17" t="s">
         <v>65</v>
-      </c>
-      <c r="H17">
-        <v>21112</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1728459672865</v>
       </c>
       <c r="J17" t="s">
         <v>66</v>
       </c>
-      <c r="K17" t="s">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="L17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="G18">
+        <v>21106</v>
+      </c>
+      <c r="H18">
+        <v>1728459673019</v>
+      </c>
+      <c r="I18" t="s">
         <v>68</v>
-      </c>
-      <c r="H18">
-        <v>21106</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1728459673019</v>
       </c>
       <c r="J18" t="s">
         <v>69</v>
       </c>
-      <c r="K18" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>70</v>
       </c>
-      <c r="L18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
         <v>97</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19">
+        <v>20149</v>
+      </c>
+      <c r="H19">
+        <v>1728459673170</v>
+      </c>
+      <c r="I19" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19">
-        <v>20149</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1728459673170</v>
       </c>
       <c r="J19" t="s">
         <v>72</v>
       </c>
-      <c r="K19" t="s">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
         <v>73</v>
       </c>
-      <c r="L19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
       <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" t="s">
         <v>74</v>
       </c>
-      <c r="F20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>210060</v>
+      </c>
+      <c r="H20">
+        <v>1728459673323</v>
+      </c>
+      <c r="I20" t="s">
         <v>75</v>
-      </c>
-      <c r="H20">
-        <v>210060</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1728459673323</v>
       </c>
       <c r="J20" t="s">
         <v>76</v>
       </c>
-      <c r="K20" t="s">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
         <v>77</v>
       </c>
-      <c r="L20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <v>21118</v>
+      </c>
+      <c r="H21">
+        <v>1728459673479</v>
+      </c>
+      <c r="I21" t="s">
         <v>78</v>
-      </c>
-      <c r="H21">
-        <v>21118</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1728459673479</v>
       </c>
       <c r="J21" t="s">
         <v>79</v>
       </c>
-      <c r="K21" t="s">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
         <v>80</v>
       </c>
-      <c r="L21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="G22">
+        <v>21244</v>
+      </c>
+      <c r="H22">
+        <v>1728459673632</v>
+      </c>
+      <c r="I22" t="s">
         <v>81</v>
-      </c>
-      <c r="H22">
-        <v>21244</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1728459673632</v>
       </c>
       <c r="J22" t="s">
         <v>82</v>
       </c>
-      <c r="K22" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
         <v>83</v>
       </c>
-      <c r="L22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
       <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <v>210054</v>
+      </c>
+      <c r="H23">
+        <v>1728459673787</v>
+      </c>
+      <c r="I23" t="s">
         <v>85</v>
-      </c>
-      <c r="H23">
-        <v>210054</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1728459673787</v>
       </c>
       <c r="J23" t="s">
         <v>86</v>
       </c>
-      <c r="K23" t="s">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
         <v>87</v>
       </c>
-      <c r="L23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="G24">
+        <v>210055</v>
+      </c>
+      <c r="H24">
+        <v>1728459673970</v>
+      </c>
+      <c r="I24" t="s">
         <v>88</v>
-      </c>
-      <c r="H24">
-        <v>210055</v>
-      </c>
-      <c r="I24" s="1">
-        <v>1728459673970</v>
       </c>
       <c r="J24" t="s">
         <v>89</v>
       </c>
-      <c r="K24" t="s">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" t="s">
         <v>90</v>
       </c>
-      <c r="L24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="G25">
+        <v>21122</v>
+      </c>
+      <c r="H25">
+        <v>1728459674122</v>
+      </c>
+      <c r="I25" t="s">
         <v>91</v>
-      </c>
-      <c r="H25">
-        <v>21122</v>
-      </c>
-      <c r="I25" s="1">
-        <v>1728459674122</v>
       </c>
       <c r="J25" t="s">
         <v>92</v>
       </c>
-      <c r="K25" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>93</v>
       </c>
-      <c r="L25" t="s">
-        <v>107</v>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>